<commit_message>
hotfix: mileage register excel file edit
</commit_message>
<xml_diff>
--- a/src/assets/mileage_register.xlsx
+++ b/src/assets/mileage_register.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeongseogmin/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sungjinpark/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480DE7B3-6F01-614A-A867-32FC69E4BDCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A3CEE6-E644-4849-B71D-DB57F5B5D04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11960" yWindow="4660" windowWidth="23560" windowHeight="16940" xr2:uid="{8CB8718E-13EB-3643-B6C4-930D62CF2B8D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="44">
   <si>
     <t>Category 번호</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -49,14 +49,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>시작날짜</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>종료날짜</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>가중치</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -113,10 +105,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2022-09-28 20:08</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -138,34 +126,6 @@
   </si>
   <si>
     <t>5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2022-09-28 21:08</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2022-09-28 23:10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2022-09-28 23:13</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2022-09-28 14:08</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2022-09-27 20:08</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2022-09-29 20:08</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2022-10-01 20:08</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -617,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1FABC25-6AA0-CF40-BE23-44E2FD0DFEE5}">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -628,13 +588,12 @@
     <col min="1" max="1" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.7109375" style="1"/>
-    <col min="12" max="12" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.7109375" style="1"/>
+    <col min="10" max="10" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -650,320 +609,242 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
+        <v>18</v>
+      </c>
+      <c r="K3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
+        <v>18</v>
+      </c>
+      <c r="K4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="1">
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="1">
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="1">
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="1">
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L8" t="s">
-        <v>11</v>
-      </c>
-      <c r="M8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
+        <v>18</v>
+      </c>
+      <c r="J8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="1">
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="1">
         <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" t="s">
         <v>2</v>
       </c>
-      <c r="M10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="K10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="1">
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="1">
         <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L12" t="s">
-        <v>18</v>
-      </c>
-      <c r="M12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="E13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>